<commit_message>
removed default client from excel file
</commit_message>
<xml_diff>
--- a/Client-Template/clientFile.xlsx
+++ b/Client-Template/clientFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Client Info" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>COMPANY</t>
   </si>
@@ -56,30 +56,6 @@
   </si>
   <si>
     <t>PROJECT</t>
-  </si>
-  <si>
-    <t>Goood Media</t>
-  </si>
-  <si>
-    <t>Johnny Rivera</t>
-  </si>
-  <si>
-    <t>71 Collingwood Dr Warwick, RI 02886</t>
-  </si>
-  <si>
-    <t>http://gooodmedia.com</t>
-  </si>
-  <si>
-    <t>hello@goodmedia.com</t>
-  </si>
-  <si>
-    <t>401-466-4459</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>goodmedia.com</t>
   </si>
   <si>
     <t>WEBSITE</t>
@@ -554,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -579,7 +555,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
@@ -598,30 +574,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -652,12 +608,8 @@
     <row r="29" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -720,7 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -736,85 +688,85 @@
   <sheetData>
     <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="10" t="s">
         <v>24</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>2</v>

</xml_diff>